<commit_message>
01/03/2023 * Uses an external clock at 62.5MHz for the processing * Uses the OK clock at 200MHz to manage the reset * Sync signal is shorter than Trow to allow Mux Factor = 1 * Clock signals renamed
</commit_message>
<xml_diff>
--- a/doc/pin_allocation.xlsx
+++ b/doc/pin_allocation.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25308"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ATHENA_X-IFU\Documents\Noemie2020\Documents_projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9794F29-709B-48C8-BD8F-23683B5A8E1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{87854248-8FC5-4F7A-B15D-F2D4E4C017B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="ras-a75-fw_005" sheetId="1" r:id="rId1"/>
+    <sheet name="ras-a75-fw_00F" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="125">
   <si>
     <t>Signaux</t>
   </si>
@@ -100,45 +100,45 @@
     <t>o_sig_overlap(0)</t>
   </si>
   <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>MC1-19</t>
+  </si>
+  <si>
+    <t>o_sig_overlap(12)</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>AA6</t>
+  </si>
+  <si>
+    <t>o_sig_overlap(1)</t>
+  </si>
+  <si>
+    <t>Y9</t>
+  </si>
+  <si>
+    <t>MC1-17</t>
+  </si>
+  <si>
+    <t>o_sig_overlap(11)</t>
+  </si>
+  <si>
+    <t>Y3</t>
+  </si>
+  <si>
+    <t>AA8</t>
+  </si>
+  <si>
+    <t>o_sig_overlap(2)</t>
+  </si>
+  <si>
     <t>W9</t>
   </si>
   <si>
-    <t>MC1-19</t>
-  </si>
-  <si>
-    <t>o_sig_overlap(12)</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>AA6</t>
-  </si>
-  <si>
-    <t>o_sig_overlap(1)</t>
-  </si>
-  <si>
-    <t>Y9</t>
-  </si>
-  <si>
-    <t>MC1-17</t>
-  </si>
-  <si>
-    <t>o_sig_overlap(11)</t>
-  </si>
-  <si>
-    <t>Y3</t>
-  </si>
-  <si>
-    <t>AA8</t>
-  </si>
-  <si>
-    <t>o_sig_overlap(2)</t>
-  </si>
-  <si>
-    <t>R6</t>
-  </si>
-  <si>
     <t>MC1-15</t>
   </si>
   <si>
@@ -386,6 +386,9 @@
   </si>
   <si>
     <t>MC1-57</t>
+  </si>
+  <si>
+    <t>o_clk</t>
   </si>
   <si>
     <t>V4</t>
@@ -771,7 +774,7 @@
   <dimension ref="A1:S37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1188,7 +1191,7 @@
         <v>32</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="J11" s="1">
         <v>15</v>
@@ -1282,7 +1285,7 @@
         <v>20</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="J13" s="1">
         <v>19</v>
@@ -1724,10 +1727,10 @@
         <v>17</v>
       </c>
       <c r="M22" s="6" t="s">
-        <v>16</v>
+        <v>117</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="Q22" s="1">
         <v>37</v>
@@ -1754,7 +1757,7 @@
         <v>34</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>74</v>
@@ -1775,7 +1778,7 @@
         <v>107</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="Q23" s="1">
         <v>39</v>
@@ -1802,7 +1805,7 @@
         <v>34</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" spans="1:19">
@@ -1822,7 +1825,7 @@
         <v>34</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:19">
@@ -1842,18 +1845,18 @@
         <v>34</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:19">
       <c r="A28" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B28" s="5"/>
     </row>
     <row r="29" spans="1:19">
       <c r="A29" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B29" s="5"/>
     </row>

</xml_diff>